<commit_message>
milan khadka sir ko kalimasta mandir ko slope design and estimate sakeko for discussing with himself
</commit_message>
<xml_diff>
--- a/ofc/estimates/khulaltaar dhikurepaati/khulaltaar dhikurepaati .xlsx
+++ b/ofc/estimates/khulaltaar dhikurepaati/khulaltaar dhikurepaati .xlsx
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -243,7 +243,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +339,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -414,7 +442,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -500,6 +528,31 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -507,9 +560,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -519,27 +569,32 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1211,8 +1266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="O58" sqref="O58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,113 +1290,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
     </row>
     <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="40" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40"/>
-      <c r="K6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="40" t="s">
+      <c r="H7" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -2330,16 +2385,16 @@
       <c r="C50" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="49" t="s">
+      <c r="D50" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E50" s="50" t="s">
+      <c r="E50" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="F50" s="50" t="s">
+      <c r="F50" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="G50" s="51" t="s">
+      <c r="G50" s="39" t="s">
         <v>54</v>
       </c>
       <c r="H50" s="25"/>
@@ -2481,11 +2536,26 @@
       <c r="B55" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C55" s="22"/>
-      <c r="D55" s="23"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="27"/>
+      <c r="C55" s="22">
+        <f>5*C40</f>
+        <v>40</v>
+      </c>
+      <c r="D55" s="23">
+        <f>D40+2*0.72</f>
+        <v>4.3863578177384941</v>
+      </c>
+      <c r="E55" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F55" s="24">
+        <f>PRODUCT(C55:E55)</f>
+        <v>155.95938907514645</v>
+      </c>
+      <c r="G55" s="27">
+        <f>F55/1000</f>
+        <v>0.15595938907514645</v>
+      </c>
       <c r="H55" s="25"/>
       <c r="I55" s="26"/>
       <c r="J55" s="27"/>
@@ -2494,28 +2564,72 @@
     <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="21"/>
       <c r="B56" s="35"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="23"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="27"/>
+      <c r="C56" s="22">
+        <f>5*C41</f>
+        <v>30</v>
+      </c>
+      <c r="D56" s="23">
+        <f>D41+2*0.72</f>
+        <v>4.3354587016153605</v>
+      </c>
+      <c r="E56" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F56" s="24">
+        <f>PRODUCT(C56:E56)</f>
+        <v>115.61223204307626</v>
+      </c>
+      <c r="G56" s="27">
+        <f>F56/1000</f>
+        <v>0.11561223204307626</v>
+      </c>
       <c r="H56" s="25"/>
       <c r="I56" s="26"/>
       <c r="J56" s="27"/>
       <c r="K56" s="24"/>
     </row>
-    <row r="57" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21"/>
-      <c r="B57" s="35"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="25"/>
-      <c r="I57" s="26"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="24"/>
+    <row r="57" spans="1:15" s="60" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="52"/>
+      <c r="B57" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="54">
+        <f>6*15</f>
+        <v>90</v>
+      </c>
+      <c r="D57" s="55">
+        <f>(0.23*4+0.05*2)</f>
+        <v>1.02</v>
+      </c>
+      <c r="E57" s="56">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F57" s="56">
+        <f t="shared" ref="F57" si="5">PRODUCT(C57:E57)</f>
+        <v>36.266666666666666</v>
+      </c>
+      <c r="G57" s="57">
+        <f t="shared" ref="G57" si="6">F57/1000</f>
+        <v>3.6266666666666662E-2</v>
+      </c>
+      <c r="H57" s="58"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="57"/>
+      <c r="K57" s="56"/>
+      <c r="M57" s="60">
+        <f>12*60</f>
+        <v>720</v>
+      </c>
+      <c r="N57" s="60">
+        <f>1.333/3.281*1000</f>
+        <v>406.27857360560802</v>
+      </c>
+      <c r="O57" s="60">
+        <f>M57-N57</f>
+        <v>313.72142639439198</v>
+      </c>
     </row>
     <row r="58" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="21"/>
@@ -2698,11 +2812,11 @@
       <c r="B68" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C68" s="37">
+      <c r="C68" s="46">
         <f>J66</f>
         <v>362160.04704907379</v>
       </c>
-      <c r="D68" s="38"/>
+      <c r="D68" s="47"/>
       <c r="E68" s="10">
         <v>100</v>
       </c>
@@ -2736,10 +2850,10 @@
       <c r="B69" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="41">
+      <c r="C69" s="49">
         <v>400000</v>
       </c>
-      <c r="D69" s="42"/>
+      <c r="D69" s="50"/>
       <c r="E69" s="10"/>
       <c r="M69" s="28"/>
       <c r="N69" s="29"/>
@@ -2765,11 +2879,11 @@
       <c r="B70" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="41">
+      <c r="C70" s="49">
         <f>C69-C72-C73</f>
         <v>380000</v>
       </c>
-      <c r="D70" s="42"/>
+      <c r="D70" s="50"/>
       <c r="E70" s="10">
         <f>C70/C68*100</f>
         <v>104.92598592701997</v>
@@ -2798,11 +2912,11 @@
       <c r="B71" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="43">
+      <c r="C71" s="51">
         <f>C68-C70</f>
         <v>-17839.952950926207</v>
       </c>
-      <c r="D71" s="43"/>
+      <c r="D71" s="51"/>
       <c r="E71" s="10">
         <f>100-E70</f>
         <v>-4.9259859270199655</v>
@@ -2831,11 +2945,11 @@
       <c r="B72" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="37">
+      <c r="C72" s="46">
         <f>C69*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D72" s="38"/>
+      <c r="D72" s="47"/>
       <c r="E72" s="10">
         <v>3</v>
       </c>
@@ -2863,11 +2977,11 @@
       <c r="B73" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C73" s="37">
+      <c r="C73" s="46">
         <f>C69*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D73" s="38"/>
+      <c r="D73" s="47"/>
       <c r="E73" s="10">
         <v>2</v>
       </c>
@@ -2893,13 +3007,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="C73:D73"/>
     <mergeCell ref="A7:F7"/>
@@ -2908,6 +3015,13 @@
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
valuation of kalimasta give to user committee
</commit_message>
<xml_diff>
--- a/ofc/estimates/khulaltaar dhikurepaati/khulaltaar dhikurepaati .xlsx
+++ b/ofc/estimates/khulaltaar dhikurepaati/khulaltaar dhikurepaati .xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\khulaltaar dhikurepaati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\khulaltaar dhikurepaati\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="18" r:id="rId1"/>
@@ -46,7 +46,7 @@
     <definedName name="skilled_blacksmith">[1]District_Rate!$D$149</definedName>
     <definedName name="unskilled">[1]District_Rate!$D$156</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -256,10 +256,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -431,9 +431,9 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -444,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,7 +452,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -469,7 +469,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,7 +478,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -490,7 +490,7 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,6 +543,22 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,9 +566,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -561,19 +574,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1245,139 +1245,139 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="52" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="53" t="s">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="53" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="47"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="54" t="s">
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="47"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="46" t="s">
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="46"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="46" t="s">
+      <c r="H7" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -1429,7 +1429,7 @@
       <c r="J9" s="27"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="21"/>
       <c r="B10" s="35" t="s">
         <v>30</v>
@@ -1455,7 +1455,7 @@
       <c r="J10" s="27"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="21"/>
       <c r="B11" s="35" t="s">
         <v>24</v>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="21"/>
       <c r="B12" s="35"/>
       <c r="C12" s="22"/>
@@ -1493,7 +1493,7 @@
       <c r="J12" s="27"/>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>2</v>
       </c>
@@ -1510,7 +1510,7 @@
       <c r="J13" s="27"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21"/>
       <c r="B14" s="35" t="s">
         <v>30</v>
@@ -1539,7 +1539,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="21"/>
       <c r="B15" s="35" t="s">
         <v>40</v>
@@ -1567,7 +1567,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21"/>
       <c r="B16" s="35" t="s">
         <v>24</v>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="K16" s="24"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21"/>
       <c r="B17" s="35" t="s">
         <v>28</v>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21"/>
       <c r="B18" s="35"/>
       <c r="C18" s="22"/>
@@ -1623,7 +1623,7 @@
       <c r="J18" s="27"/>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>3</v>
       </c>
@@ -1640,7 +1640,7 @@
       <c r="J19" s="27"/>
       <c r="K19" s="24"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="21"/>
       <c r="B20" s="35" t="s">
         <v>30</v>
@@ -1669,7 +1669,7 @@
       <c r="J20" s="27"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21"/>
       <c r="B21" s="35" t="s">
         <v>24</v>
@@ -1694,7 +1694,7 @@
       </c>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21"/>
       <c r="B22" s="35" t="s">
         <v>28</v>
@@ -1712,7 +1712,7 @@
       </c>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21"/>
       <c r="B23" s="35"/>
       <c r="C23" s="22"/>
@@ -1725,7 +1725,7 @@
       <c r="J23" s="27"/>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>4</v>
       </c>
@@ -1742,7 +1742,7 @@
       <c r="J24" s="27"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="35" t="str">
         <f>B20</f>
@@ -1770,7 +1770,7 @@
       <c r="J25" s="27"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21"/>
       <c r="B26" s="35" t="s">
         <v>38</v>
@@ -1796,7 +1796,7 @@
       <c r="J26" s="27"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="35" t="s">
         <v>39</v>
@@ -1823,7 +1823,7 @@
       <c r="J27" s="27"/>
       <c r="K27" s="24"/>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21"/>
       <c r="B28" s="35"/>
       <c r="C28" s="22">
@@ -1848,7 +1848,7 @@
       <c r="J28" s="27"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
       <c r="B29" s="35" t="s">
         <v>41</v>
@@ -1875,14 +1875,14 @@
       <c r="J29" s="27"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21"/>
       <c r="B30" s="35" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="22">
-        <f>4</f>
-        <v>4</v>
+        <f>0*4</f>
+        <v>0</v>
       </c>
       <c r="D30" s="23">
         <f>9.667/3.281</f>
@@ -1895,19 +1895,19 @@
       </c>
       <c r="G30" s="33">
         <f t="shared" ref="G30:G32" si="1">PRODUCT(C30:F30)</f>
-        <v>5.4212983846388294</v>
+        <v>0</v>
       </c>
       <c r="H30" s="25"/>
       <c r="I30" s="26"/>
       <c r="J30" s="27"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21"/>
       <c r="B31" s="35"/>
       <c r="C31" s="22">
-        <f>3</f>
-        <v>3</v>
+        <f>0*3</f>
+        <v>0</v>
       </c>
       <c r="D31" s="23">
         <f>9.5/3.281</f>
@@ -1920,20 +1920,21 @@
       </c>
       <c r="G31" s="33">
         <f t="shared" si="1"/>
-        <v>3.9957330082291982</v>
+        <v>0</v>
       </c>
       <c r="H31" s="25"/>
       <c r="I31" s="26"/>
       <c r="J31" s="27"/>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="21"/>
       <c r="B32" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="22">
-        <v>1</v>
+        <f>0*1</f>
+        <v>0</v>
       </c>
       <c r="D32" s="23">
         <f>(22.333+3)/3.281</f>
@@ -1946,14 +1947,14 @@
       <c r="F32" s="24"/>
       <c r="G32" s="33">
         <f t="shared" si="1"/>
-        <v>34.122603881240252</v>
+        <v>0</v>
       </c>
       <c r="H32" s="25"/>
       <c r="I32" s="26"/>
       <c r="J32" s="27"/>
       <c r="K32" s="24"/>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="35" t="s">
         <v>24</v>
@@ -1964,7 +1965,7 @@
       <c r="F33" s="24"/>
       <c r="G33" s="27">
         <f>SUM(G25:G32)</f>
-        <v>96.262963527689507</v>
+        <v>52.723328253581229</v>
       </c>
       <c r="H33" s="25" t="s">
         <v>25</v>
@@ -1974,11 +1975,11 @@
       </c>
       <c r="J33" s="27">
         <f>G33*I33</f>
-        <v>88121.042072517521</v>
+        <v>48263.989149893328</v>
       </c>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21"/>
       <c r="B34" s="35" t="s">
         <v>28</v>
@@ -1992,11 +1993,11 @@
       <c r="I34" s="26"/>
       <c r="J34" s="27">
         <f>0.13*G33*46827.87/100</f>
-        <v>5860.1264044562013</v>
+        <v>3209.5975098538374</v>
       </c>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="21"/>
       <c r="B35" s="35"/>
       <c r="C35" s="22"/>
@@ -2009,7 +2010,7 @@
       <c r="J35" s="27"/>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="21">
         <v>5</v>
       </c>
@@ -2026,7 +2027,7 @@
       <c r="J36" s="27"/>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="35" t="str">
         <f>B25</f>
@@ -2055,7 +2056,7 @@
       <c r="J37" s="27"/>
       <c r="K37" s="24"/>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="21"/>
       <c r="B38" s="35"/>
       <c r="C38" s="22">
@@ -2081,7 +2082,7 @@
       <c r="J38" s="27"/>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="21"/>
       <c r="B39" s="35" t="s">
         <v>44</v>
@@ -2107,7 +2108,7 @@
       <c r="J39" s="27"/>
       <c r="K39" s="24"/>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="21"/>
       <c r="B40" s="35" t="s">
         <v>39</v>
@@ -2135,7 +2136,7 @@
       <c r="J40" s="27"/>
       <c r="K40" s="24"/>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21"/>
       <c r="B41" s="35"/>
       <c r="C41" s="22">
@@ -2161,7 +2162,7 @@
       <c r="J41" s="27"/>
       <c r="K41" s="24"/>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21"/>
       <c r="B42" s="35" t="s">
         <v>40</v>
@@ -2189,7 +2190,7 @@
       <c r="J42" s="27"/>
       <c r="K42" s="24"/>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="21"/>
       <c r="B43" s="35" t="s">
         <v>45</v>
@@ -2217,13 +2218,14 @@
       <c r="J43" s="27"/>
       <c r="K43" s="24"/>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="21"/>
       <c r="B44" s="35" t="s">
         <v>46</v>
       </c>
       <c r="C44" s="22">
-        <v>4</v>
+        <f>0*4</f>
+        <v>0</v>
       </c>
       <c r="D44" s="23">
         <f>D40</f>
@@ -2237,18 +2239,19 @@
       </c>
       <c r="G44" s="33">
         <f t="shared" si="2"/>
-        <v>0.62344931423346539</v>
+        <v>0</v>
       </c>
       <c r="H44" s="25"/>
       <c r="I44" s="26"/>
       <c r="J44" s="27"/>
       <c r="K44" s="24"/>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21"/>
       <c r="B45" s="35"/>
       <c r="C45" s="22">
-        <v>3</v>
+        <f>0*3</f>
+        <v>0</v>
       </c>
       <c r="D45" s="23">
         <f>D41</f>
@@ -2262,20 +2265,21 @@
       </c>
       <c r="G45" s="33">
         <f t="shared" si="2"/>
-        <v>0.45950929594635781</v>
+        <v>0</v>
       </c>
       <c r="H45" s="25"/>
       <c r="I45" s="26"/>
       <c r="J45" s="27"/>
       <c r="K45" s="24"/>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21"/>
       <c r="B46" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C46" s="22">
-        <v>1</v>
+        <f>0*1</f>
+        <v>0</v>
       </c>
       <c r="D46" s="23">
         <f>D32</f>
@@ -2291,14 +2295,14 @@
       </c>
       <c r="G46" s="33">
         <f t="shared" si="2"/>
-        <v>4.3333592249873334</v>
+        <v>0</v>
       </c>
       <c r="H46" s="25"/>
       <c r="I46" s="26"/>
       <c r="J46" s="27"/>
       <c r="K46" s="24"/>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="21"/>
       <c r="B47" s="35" t="s">
         <v>24</v>
@@ -2309,7 +2313,7 @@
       <c r="F47" s="24"/>
       <c r="G47" s="27">
         <f>SUM(G37:G46)</f>
-        <v>14.608959623239278</v>
+        <v>9.1926417880721214</v>
       </c>
       <c r="H47" s="25" t="s">
         <v>31</v>
@@ -2319,11 +2323,11 @@
       </c>
       <c r="J47" s="27">
         <f>G47*I47</f>
-        <v>198227.51223177143</v>
+        <v>124734.03715817181</v>
       </c>
       <c r="K47" s="24"/>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="21"/>
       <c r="B48" s="35" t="s">
         <v>28</v>
@@ -2337,11 +2341,11 @@
       <c r="I48" s="26"/>
       <c r="J48" s="27">
         <f>0.13*G47*9524.2</f>
-        <v>18088.02492167522</v>
+        <v>11381.832659334344</v>
       </c>
       <c r="K48" s="24"/>
     </row>
-    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="21"/>
       <c r="B49" s="35"/>
       <c r="C49" s="22"/>
@@ -2354,7 +2358,7 @@
       <c r="J49" s="27"/>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" spans="1:15" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="21">
         <v>6</v>
       </c>
@@ -2381,7 +2385,7 @@
       <c r="J50" s="27"/>
       <c r="K50" s="24"/>
     </row>
-    <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="21"/>
       <c r="B51" s="35" t="s">
         <v>48</v>
@@ -2410,7 +2414,7 @@
       <c r="J51" s="27"/>
       <c r="K51" s="24"/>
     </row>
-    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="21"/>
       <c r="B52" s="35" t="s">
         <v>54</v>
@@ -2440,7 +2444,7 @@
       <c r="J52" s="27"/>
       <c r="K52" s="24"/>
     </row>
-    <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="21"/>
       <c r="B53" s="35" t="s">
         <v>55</v>
@@ -2482,7 +2486,7 @@
         <v>313.72142639439198</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21"/>
       <c r="B54" s="35"/>
       <c r="C54" s="22">
@@ -2510,7 +2514,7 @@
       <c r="J54" s="27"/>
       <c r="K54" s="24"/>
     </row>
-    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="21"/>
       <c r="B55" s="35" t="s">
         <v>56</v>
@@ -2540,7 +2544,7 @@
       <c r="J55" s="27"/>
       <c r="K55" s="24"/>
     </row>
-    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="21"/>
       <c r="B56" s="35"/>
       <c r="C56" s="22">
@@ -2568,7 +2572,7 @@
       <c r="J56" s="27"/>
       <c r="K56" s="24"/>
     </row>
-    <row r="57" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="21"/>
       <c r="B57" s="40" t="s">
         <v>55</v>
@@ -2610,7 +2614,7 @@
         <v>313.72142639439198</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
       <c r="B58" s="40"/>
       <c r="C58" s="22">
@@ -2638,13 +2642,14 @@
       <c r="J58" s="41"/>
       <c r="K58" s="24"/>
     </row>
-    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21"/>
       <c r="B59" s="35" t="s">
         <v>46</v>
       </c>
       <c r="C59" s="22">
-        <v>2</v>
+        <f>0*2</f>
+        <v>0</v>
       </c>
       <c r="D59" s="23">
         <f>(20.333/3.281)+0.72*2</f>
@@ -2656,22 +2661,23 @@
       </c>
       <c r="F59" s="24">
         <f t="shared" ref="F59:F61" si="9">PRODUCT(C59:E59)</f>
-        <v>13.577237292153473</v>
+        <v>0</v>
       </c>
       <c r="G59" s="41">
         <f t="shared" ref="G59:G61" si="10">F59/1000</f>
-        <v>1.3577237292153474E-2</v>
+        <v>0</v>
       </c>
       <c r="H59" s="25"/>
       <c r="I59" s="26"/>
       <c r="J59" s="27"/>
       <c r="K59" s="24"/>
     </row>
-    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="21"/>
       <c r="B60" s="35"/>
       <c r="C60" s="22">
-        <v>3</v>
+        <f>0*3</f>
+        <v>0</v>
       </c>
       <c r="D60" s="23">
         <f>(9.5/3.281)+0.72*2</f>
@@ -2683,25 +2689,25 @@
       </c>
       <c r="F60" s="24">
         <f t="shared" si="9"/>
-        <v>11.561223204307627</v>
+        <v>0</v>
       </c>
       <c r="G60" s="41">
         <f t="shared" si="10"/>
-        <v>1.1561223204307627E-2</v>
+        <v>0</v>
       </c>
       <c r="H60" s="25"/>
       <c r="I60" s="26"/>
       <c r="J60" s="27"/>
       <c r="K60" s="24"/>
     </row>
-    <row r="61" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="21"/>
       <c r="B61" s="40" t="s">
         <v>55</v>
       </c>
       <c r="C61" s="22">
-        <f>2*TRUNC((D59-3*0.72)/0.125,0)</f>
-        <v>86</v>
+        <f>0*2*TRUNC((D59-3*0.72)/0.125,0)</f>
+        <v>0</v>
       </c>
       <c r="D61" s="23">
         <f>(0.23*2+0.15*2+0.05*2)</f>
@@ -2713,11 +2719,11 @@
       </c>
       <c r="F61" s="24">
         <f t="shared" si="9"/>
-        <v>29.21876543209876</v>
+        <v>0</v>
       </c>
       <c r="G61" s="41">
         <f t="shared" si="10"/>
-        <v>2.921876543209876E-2</v>
+        <v>0</v>
       </c>
       <c r="H61" s="25"/>
       <c r="I61" s="26"/>
@@ -2736,12 +2742,12 @@
         <v>313.72142639439198</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
       <c r="B62" s="35"/>
       <c r="C62" s="22">
-        <f>3*TRUNC((D60-2*0.72)/0.125,0)</f>
-        <v>69</v>
+        <f>0*3*TRUNC((D60-2*0.72)/0.125,0)</f>
+        <v>0</v>
       </c>
       <c r="D62" s="23">
         <f>(0.23*2+0.15*2+0.05*2)</f>
@@ -2753,25 +2759,25 @@
       </c>
       <c r="F62" s="24">
         <f t="shared" ref="F62" si="11">PRODUCT(C62:E62)</f>
-        <v>23.442962962962959</v>
+        <v>0</v>
       </c>
       <c r="G62" s="41">
         <f t="shared" ref="G62" si="12">F62/1000</f>
-        <v>2.3442962962962957E-2</v>
+        <v>0</v>
       </c>
       <c r="H62" s="25"/>
       <c r="I62" s="26"/>
       <c r="J62" s="27"/>
       <c r="K62" s="24"/>
     </row>
-    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
       <c r="B63" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C63" s="22">
-        <f>TRUNC(12.5/0.5,0)+1</f>
-        <v>26</v>
+        <f>0*TRUNC(12.5/0.5,0)+1</f>
+        <v>1</v>
       </c>
       <c r="D63" s="23">
         <f>25/3.281</f>
@@ -2783,23 +2789,23 @@
       </c>
       <c r="F63" s="24">
         <f t="shared" ref="F63" si="13">PRODUCT(C63:E63)</f>
-        <v>78.265810258089019</v>
+        <v>3.0102234714649625</v>
       </c>
       <c r="G63" s="41">
         <f t="shared" ref="G63" si="14">F63/1000</f>
-        <v>7.8265810258089014E-2</v>
+        <v>3.0102234714649624E-3</v>
       </c>
       <c r="H63" s="25"/>
       <c r="I63" s="26"/>
       <c r="J63" s="27"/>
       <c r="K63" s="24"/>
     </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="21"/>
       <c r="B64" s="35"/>
       <c r="C64" s="22">
-        <f>TRUNC((25.333-0.333-0.75*3)/0.5,0)+1</f>
-        <v>46</v>
+        <f>0*TRUNC((25.333-0.333-0.75*3)/0.5,0)+1</f>
+        <v>1</v>
       </c>
       <c r="D64" s="23">
         <f>14.17/3.281</f>
@@ -2811,24 +2817,25 @@
       </c>
       <c r="F64" s="24">
         <f>PRODUCT(C64:E64)</f>
-        <v>78.484954526811677</v>
+        <v>1.7061946636263408</v>
       </c>
       <c r="G64" s="41">
         <f>F64/1000</f>
-        <v>7.8484954526811673E-2</v>
+        <v>1.7061946636263408E-3</v>
       </c>
       <c r="H64" s="25"/>
       <c r="I64" s="26"/>
       <c r="J64" s="27"/>
       <c r="K64" s="24"/>
     </row>
-    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="21"/>
       <c r="B65" s="35" t="s">
         <v>58</v>
       </c>
       <c r="C65" s="22">
-        <v>30</v>
+        <f>0*30</f>
+        <v>0</v>
       </c>
       <c r="D65" s="23">
         <f>14.17/3.281</f>
@@ -2840,23 +2847,23 @@
       </c>
       <c r="F65" s="24">
         <f t="shared" ref="F65:F66" si="16">PRODUCT(C65:E65)</f>
-        <v>51.185839908790221</v>
+        <v>0</v>
       </c>
       <c r="G65" s="41">
         <f t="shared" ref="G65:G66" si="17">F65/1000</f>
-        <v>5.118583990879022E-2</v>
+        <v>0</v>
       </c>
       <c r="H65" s="25"/>
       <c r="I65" s="26"/>
       <c r="J65" s="27"/>
       <c r="K65" s="24"/>
     </row>
-    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21"/>
       <c r="B66" s="35"/>
       <c r="C66" s="22">
-        <f>9*2</f>
-        <v>18</v>
+        <f>0*9*2</f>
+        <v>0</v>
       </c>
       <c r="D66" s="23">
         <f>25/3.281</f>
@@ -2868,25 +2875,25 @@
       </c>
       <c r="F66" s="24">
         <f t="shared" si="16"/>
-        <v>54.184022486369322</v>
+        <v>0</v>
       </c>
       <c r="G66" s="41">
         <f t="shared" si="17"/>
-        <v>5.4184022486369325E-2</v>
+        <v>0</v>
       </c>
       <c r="H66" s="25"/>
       <c r="I66" s="26"/>
       <c r="J66" s="27"/>
       <c r="K66" s="24"/>
     </row>
-    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21"/>
       <c r="B67" s="35" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="22">
-        <f>7*4</f>
-        <v>28</v>
+        <f>0*7*4</f>
+        <v>0</v>
       </c>
       <c r="D67" s="23">
         <f>1.5</f>
@@ -2898,11 +2905,11 @@
       </c>
       <c r="F67" s="24">
         <f t="shared" ref="F67:F69" si="19">PRODUCT(C67:E67)</f>
-        <v>16.592592592592592</v>
+        <v>0</v>
       </c>
       <c r="G67" s="41">
         <f t="shared" ref="G67:G69" si="20">F67/1000</f>
-        <v>1.6592592592592593E-2</v>
+        <v>0</v>
       </c>
       <c r="H67" s="25"/>
       <c r="I67" s="26"/>
@@ -2913,11 +2920,12 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21"/>
       <c r="B68" s="35"/>
       <c r="C68" s="22">
-        <v>16</v>
+        <f>0*16</f>
+        <v>0</v>
       </c>
       <c r="D68" s="23">
         <f>5.333/3.281</f>
@@ -2929,22 +2937,23 @@
       </c>
       <c r="F68" s="24">
         <f t="shared" si="19"/>
-        <v>10.274253934926493</v>
+        <v>0</v>
       </c>
       <c r="G68" s="41">
         <f t="shared" si="20"/>
-        <v>1.0274253934926493E-2</v>
+        <v>0</v>
       </c>
       <c r="H68" s="25"/>
       <c r="I68" s="26"/>
       <c r="J68" s="27"/>
       <c r="K68" s="24"/>
     </row>
-    <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="35"/>
       <c r="C69" s="22">
-        <v>8</v>
+        <f>0*8</f>
+        <v>0</v>
       </c>
       <c r="D69" s="23">
         <f>7.25/3.281</f>
@@ -2956,18 +2965,18 @@
       </c>
       <c r="F69" s="24">
         <f t="shared" si="19"/>
-        <v>6.9837184537987138</v>
+        <v>0</v>
       </c>
       <c r="G69" s="41">
         <f t="shared" si="20"/>
-        <v>6.9837184537987138E-3</v>
+        <v>0</v>
       </c>
       <c r="H69" s="25"/>
       <c r="I69" s="26"/>
       <c r="J69" s="27"/>
       <c r="K69" s="24"/>
     </row>
-    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
       <c r="B70" s="35" t="s">
         <v>24</v>
@@ -2978,7 +2987,7 @@
       <c r="F70" s="24"/>
       <c r="G70" s="27">
         <f>SUM(G51:G69)</f>
-        <v>1.1590903670591244</v>
+        <v>0.7900354041413149</v>
       </c>
       <c r="H70" s="25" t="s">
         <v>62</v>
@@ -2988,11 +2997,11 @@
       </c>
       <c r="J70" s="27">
         <f>G70*I70</f>
-        <v>152930.38302978087</v>
+        <v>104237.27122240509</v>
       </c>
       <c r="K70" s="24"/>
     </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
       <c r="B71" s="35" t="s">
         <v>28</v>
@@ -3006,11 +3015,11 @@
       <c r="I71" s="26"/>
       <c r="J71" s="27">
         <f>0.13*G70*106200</f>
-        <v>16002.401607618271</v>
+        <v>10907.228789574994</v>
       </c>
       <c r="K71" s="24"/>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
       <c r="B72" s="35"/>
       <c r="C72" s="22"/>
@@ -3023,7 +3032,7 @@
       <c r="J72" s="27"/>
       <c r="K72" s="24"/>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="21">
         <v>7</v>
       </c>
@@ -3040,7 +3049,7 @@
       <c r="J73" s="27"/>
       <c r="K73" s="24"/>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="21"/>
       <c r="B74" s="35" t="s">
         <v>61</v>
@@ -3068,7 +3077,7 @@
       <c r="J74" s="27"/>
       <c r="K74" s="24"/>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
       <c r="B75" s="35"/>
       <c r="C75" s="22">
@@ -3094,7 +3103,7 @@
       <c r="J75" s="27"/>
       <c r="K75" s="24"/>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="35"/>
       <c r="C76" s="22">
@@ -3120,7 +3129,7 @@
       <c r="J76" s="27"/>
       <c r="K76" s="24"/>
     </row>
-    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="21"/>
       <c r="B77" s="35"/>
       <c r="C77" s="22">
@@ -3146,7 +3155,7 @@
       <c r="J77" s="27"/>
       <c r="K77" s="24"/>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="21"/>
       <c r="B78" s="35" t="s">
         <v>64</v>
@@ -3175,7 +3184,7 @@
       <c r="J78" s="27"/>
       <c r="K78" s="24"/>
     </row>
-    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="35" t="s">
         <v>24</v>
@@ -3200,7 +3209,7 @@
       </c>
       <c r="K79" s="24"/>
     </row>
-    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="21"/>
       <c r="B80" s="35" t="s">
         <v>28</v>
@@ -3218,7 +3227,7 @@
       </c>
       <c r="K80" s="24"/>
     </row>
-    <row r="81" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="21"/>
       <c r="B81" s="35"/>
       <c r="C81" s="22"/>
@@ -3231,7 +3240,7 @@
       <c r="J81" s="27"/>
       <c r="K81" s="24"/>
     </row>
-    <row r="82" spans="1:31" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:31" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A82" s="21">
         <v>8</v>
       </c>
@@ -3260,7 +3269,7 @@
       </c>
       <c r="K82" s="24"/>
     </row>
-    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="21"/>
       <c r="B83" s="35"/>
       <c r="C83" s="22"/>
@@ -3273,7 +3282,7 @@
       <c r="J83" s="27"/>
       <c r="K83" s="24"/>
     </row>
-    <row r="84" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="21">
         <v>9</v>
       </c>
@@ -3302,7 +3311,7 @@
       </c>
       <c r="K84" s="24"/>
     </row>
-    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="21"/>
       <c r="B85" s="35"/>
       <c r="C85" s="22"/>
@@ -3315,7 +3324,7 @@
       <c r="J85" s="27"/>
       <c r="K85" s="24"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A86" s="9"/>
       <c r="B86" s="20" t="s">
         <v>16</v>
@@ -3329,14 +3338,14 @@
       <c r="I86" s="7"/>
       <c r="J86" s="7">
         <f>SUM(J9:J85)</f>
-        <v>665993.58174243139</v>
+        <v>489498.04796384519</v>
       </c>
       <c r="K86" s="4"/>
       <c r="M86" s="28"/>
       <c r="P86" s="31"/>
       <c r="Q86" s="31"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
       <c r="M87" s="28"/>
       <c r="N87" s="29"/>
       <c r="O87" s="29"/>
@@ -3356,15 +3365,15 @@
       <c r="AD87" s="28"/>
       <c r="AE87" s="28"/>
     </row>
-    <row r="88" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C88" s="43">
+      <c r="C88" s="49">
         <f>J86</f>
-        <v>665993.58174243139</v>
-      </c>
-      <c r="D88" s="44"/>
+        <v>489498.04796384519</v>
+      </c>
+      <c r="D88" s="50"/>
       <c r="E88" s="10">
         <v>100</v>
       </c>
@@ -3394,14 +3403,14 @@
       <c r="AD88" s="12"/>
       <c r="AE88" s="12"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B89" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C89" s="47">
+      <c r="C89" s="52">
         <v>400000</v>
       </c>
-      <c r="D89" s="48"/>
+      <c r="D89" s="53"/>
       <c r="E89" s="10"/>
       <c r="M89" s="28"/>
       <c r="N89" s="29"/>
@@ -3423,18 +3432,18 @@
       <c r="AD89" s="28"/>
       <c r="AE89" s="28"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B90" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="47">
+      <c r="C90" s="52">
         <f>C89-C92-C93</f>
         <v>380000</v>
       </c>
-      <c r="D90" s="48"/>
+      <c r="D90" s="53"/>
       <c r="E90" s="10">
         <f>C90/C88*100</f>
-        <v>57.057606922548764</v>
+        <v>77.63054450996853</v>
       </c>
       <c r="M90" s="28"/>
       <c r="N90" s="28"/>
@@ -3456,18 +3465,18 @@
       <c r="AD90" s="28"/>
       <c r="AE90" s="28"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B91" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C91" s="49">
+      <c r="C91" s="54">
         <f>C88-C90</f>
-        <v>285993.58174243139</v>
-      </c>
-      <c r="D91" s="49"/>
+        <v>109498.04796384519</v>
+      </c>
+      <c r="D91" s="54"/>
       <c r="E91" s="10">
         <f>100-E90</f>
-        <v>42.942393077451236</v>
+        <v>22.36945549003147</v>
       </c>
       <c r="M91" s="28"/>
       <c r="N91" s="28"/>
@@ -3489,15 +3498,15 @@
       <c r="AD91" s="28"/>
       <c r="AE91" s="28"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B92" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="43">
+      <c r="C92" s="49">
         <f>C89*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D92" s="44"/>
+      <c r="D92" s="50"/>
       <c r="E92" s="10">
         <v>3</v>
       </c>
@@ -3521,15 +3530,15 @@
       <c r="AD92" s="28"/>
       <c r="AE92" s="28"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B93" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C93" s="43">
+      <c r="C93" s="49">
         <f>C89*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D93" s="44"/>
+      <c r="D93" s="50"/>
       <c r="E93" s="10">
         <v>2</v>
       </c>
@@ -3555,13 +3564,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="C93:D93"/>
     <mergeCell ref="A7:F7"/>
@@ -3570,6 +3572,13 @@
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C91:D91"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some files and folders mngmnt
</commit_message>
<xml_diff>
--- a/ofc/estimates/khulaltaar dhikurepaati/khulaltaar dhikurepaati .xlsx
+++ b/ofc/estimates/khulaltaar dhikurepaati/khulaltaar dhikurepaati .xlsx
@@ -2,24 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\khulaltaar dhikurepaati\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\khulaltaar dhikurepaati\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="18" r:id="rId1"/>
+    <sheet name="400k" sheetId="19" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="adopted_rate_aggregate_10_20_mm">[1]District_Rate!$L$6</definedName>
@@ -40,13 +41,15 @@
     <definedName name="description_784">[2]Abstract!$B$300</definedName>
     <definedName name="excavator">[1]Equipment_Rate!$J$19</definedName>
     <definedName name="generator">[1]Equipment_Rate!$J$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'400k'!$A$1:$K$93</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">new!$A$1:$K$93</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'400k'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">new!$1:$8</definedName>
     <definedName name="skilled">[1]District_Rate!$D$148</definedName>
     <definedName name="skilled_blacksmith">[1]District_Rate!$D$149</definedName>
     <definedName name="unskilled">[1]District_Rate!$D$156</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="65">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -256,10 +259,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -431,9 +434,9 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
@@ -444,7 +447,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,7 +455,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -469,7 +472,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,7 +481,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -490,7 +493,7 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -543,10 +546,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -558,22 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1245,139 +1248,139 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="47" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="44"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="51" t="s">
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="46" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-    </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <v>1</v>
       </c>
@@ -1429,7 +1432,7 @@
       <c r="J9" s="27"/>
       <c r="K9" s="24"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="35" t="s">
         <v>30</v>
@@ -1455,7 +1458,7 @@
       <c r="J10" s="27"/>
       <c r="K10" s="24"/>
     </row>
-    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21"/>
       <c r="B11" s="35" t="s">
         <v>24</v>
@@ -1480,7 +1483,7 @@
       </c>
       <c r="K11" s="24"/>
     </row>
-    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21"/>
       <c r="B12" s="35"/>
       <c r="C12" s="22"/>
@@ -1493,7 +1496,7 @@
       <c r="J12" s="27"/>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <v>2</v>
       </c>
@@ -1510,7 +1513,7 @@
       <c r="J13" s="27"/>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21"/>
       <c r="B14" s="35" t="s">
         <v>30</v>
@@ -1539,7 +1542,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="35" t="s">
         <v>40</v>
@@ -1567,7 +1570,7 @@
       <c r="J15" s="27"/>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
       <c r="B16" s="35" t="s">
         <v>24</v>
@@ -1592,7 +1595,7 @@
       </c>
       <c r="K16" s="24"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
       <c r="B17" s="35" t="s">
         <v>28</v>
@@ -1610,7 +1613,7 @@
       </c>
       <c r="K17" s="24"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21"/>
       <c r="B18" s="35"/>
       <c r="C18" s="22"/>
@@ -1623,7 +1626,7 @@
       <c r="J18" s="27"/>
       <c r="K18" s="24"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <v>3</v>
       </c>
@@ -1640,7 +1643,7 @@
       <c r="J19" s="27"/>
       <c r="K19" s="24"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21"/>
       <c r="B20" s="35" t="s">
         <v>30</v>
@@ -1669,7 +1672,7 @@
       <c r="J20" s="27"/>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21"/>
       <c r="B21" s="35" t="s">
         <v>24</v>
@@ -1694,7 +1697,7 @@
       </c>
       <c r="K21" s="24"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
       <c r="B22" s="35" t="s">
         <v>28</v>
@@ -1712,7 +1715,7 @@
       </c>
       <c r="K22" s="24"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
       <c r="B23" s="35"/>
       <c r="C23" s="22"/>
@@ -1725,7 +1728,7 @@
       <c r="J23" s="27"/>
       <c r="K23" s="24"/>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
         <v>4</v>
       </c>
@@ -1742,7 +1745,7 @@
       <c r="J24" s="27"/>
       <c r="K24" s="24"/>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21"/>
       <c r="B25" s="35" t="str">
         <f>B20</f>
@@ -1770,7 +1773,7 @@
       <c r="J25" s="27"/>
       <c r="K25" s="24"/>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21"/>
       <c r="B26" s="35" t="s">
         <v>38</v>
@@ -1796,7 +1799,7 @@
       <c r="J26" s="27"/>
       <c r="K26" s="24"/>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21"/>
       <c r="B27" s="35" t="s">
         <v>39</v>
@@ -1823,7 +1826,7 @@
       <c r="J27" s="27"/>
       <c r="K27" s="24"/>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21"/>
       <c r="B28" s="35"/>
       <c r="C28" s="22">
@@ -1848,7 +1851,7 @@
       <c r="J28" s="27"/>
       <c r="K28" s="24"/>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
       <c r="B29" s="35" t="s">
         <v>41</v>
@@ -1875,7 +1878,7 @@
       <c r="J29" s="27"/>
       <c r="K29" s="24"/>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
       <c r="B30" s="35" t="s">
         <v>42</v>
@@ -1902,7 +1905,7 @@
       <c r="J30" s="27"/>
       <c r="K30" s="24"/>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21"/>
       <c r="B31" s="35"/>
       <c r="C31" s="22">
@@ -1927,7 +1930,7 @@
       <c r="J31" s="27"/>
       <c r="K31" s="24"/>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21"/>
       <c r="B32" s="35" t="s">
         <v>43</v>
@@ -1954,7 +1957,7 @@
       <c r="J32" s="27"/>
       <c r="K32" s="24"/>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21"/>
       <c r="B33" s="35" t="s">
         <v>24</v>
@@ -1979,7 +1982,7 @@
       </c>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21"/>
       <c r="B34" s="35" t="s">
         <v>28</v>
@@ -1997,7 +2000,7 @@
       </c>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
       <c r="B35" s="35"/>
       <c r="C35" s="22"/>
@@ -2010,7 +2013,7 @@
       <c r="J35" s="27"/>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" s="21">
         <v>5</v>
       </c>
@@ -2027,7 +2030,7 @@
       <c r="J36" s="27"/>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21"/>
       <c r="B37" s="35" t="str">
         <f>B25</f>
@@ -2056,7 +2059,7 @@
       <c r="J37" s="27"/>
       <c r="K37" s="24"/>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21"/>
       <c r="B38" s="35"/>
       <c r="C38" s="22">
@@ -2082,7 +2085,7 @@
       <c r="J38" s="27"/>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21"/>
       <c r="B39" s="35" t="s">
         <v>44</v>
@@ -2108,7 +2111,7 @@
       <c r="J39" s="27"/>
       <c r="K39" s="24"/>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21"/>
       <c r="B40" s="35" t="s">
         <v>39</v>
@@ -2136,7 +2139,7 @@
       <c r="J40" s="27"/>
       <c r="K40" s="24"/>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
       <c r="B41" s="35"/>
       <c r="C41" s="22">
@@ -2162,7 +2165,7 @@
       <c r="J41" s="27"/>
       <c r="K41" s="24"/>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="21"/>
       <c r="B42" s="35" t="s">
         <v>40</v>
@@ -2190,7 +2193,7 @@
       <c r="J42" s="27"/>
       <c r="K42" s="24"/>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="21"/>
       <c r="B43" s="35" t="s">
         <v>45</v>
@@ -2218,7 +2221,7 @@
       <c r="J43" s="27"/>
       <c r="K43" s="24"/>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="21"/>
       <c r="B44" s="35" t="s">
         <v>46</v>
@@ -2246,7 +2249,7 @@
       <c r="J44" s="27"/>
       <c r="K44" s="24"/>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="21"/>
       <c r="B45" s="35"/>
       <c r="C45" s="22">
@@ -2272,7 +2275,7 @@
       <c r="J45" s="27"/>
       <c r="K45" s="24"/>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="21"/>
       <c r="B46" s="35" t="s">
         <v>43</v>
@@ -2302,7 +2305,7 @@
       <c r="J46" s="27"/>
       <c r="K46" s="24"/>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="21"/>
       <c r="B47" s="35" t="s">
         <v>24</v>
@@ -2327,7 +2330,7 @@
       </c>
       <c r="K47" s="24"/>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="21"/>
       <c r="B48" s="35" t="s">
         <v>28</v>
@@ -2345,7 +2348,7 @@
       </c>
       <c r="K48" s="24"/>
     </row>
-    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="21"/>
       <c r="B49" s="35"/>
       <c r="C49" s="22"/>
@@ -2358,7 +2361,7 @@
       <c r="J49" s="27"/>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" spans="1:15" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="21">
         <v>6</v>
       </c>
@@ -2385,7 +2388,7 @@
       <c r="J50" s="27"/>
       <c r="K50" s="24"/>
     </row>
-    <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="21"/>
       <c r="B51" s="35" t="s">
         <v>48</v>
@@ -2414,7 +2417,7 @@
       <c r="J51" s="27"/>
       <c r="K51" s="24"/>
     </row>
-    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="21"/>
       <c r="B52" s="35" t="s">
         <v>54</v>
@@ -2444,7 +2447,7 @@
       <c r="J52" s="27"/>
       <c r="K52" s="24"/>
     </row>
-    <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21"/>
       <c r="B53" s="35" t="s">
         <v>55</v>
@@ -2486,7 +2489,7 @@
         <v>313.72142639439198</v>
       </c>
     </row>
-    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="21"/>
       <c r="B54" s="35"/>
       <c r="C54" s="22">
@@ -2514,7 +2517,7 @@
       <c r="J54" s="27"/>
       <c r="K54" s="24"/>
     </row>
-    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="21"/>
       <c r="B55" s="35" t="s">
         <v>56</v>
@@ -2544,7 +2547,7 @@
       <c r="J55" s="27"/>
       <c r="K55" s="24"/>
     </row>
-    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="21"/>
       <c r="B56" s="35"/>
       <c r="C56" s="22">
@@ -2572,7 +2575,7 @@
       <c r="J56" s="27"/>
       <c r="K56" s="24"/>
     </row>
-    <row r="57" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="21"/>
       <c r="B57" s="40" t="s">
         <v>55</v>
@@ -2614,7 +2617,7 @@
         <v>313.72142639439198</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="21"/>
       <c r="B58" s="40"/>
       <c r="C58" s="22">
@@ -2642,7 +2645,7 @@
       <c r="J58" s="41"/>
       <c r="K58" s="24"/>
     </row>
-    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="21"/>
       <c r="B59" s="35" t="s">
         <v>46</v>
@@ -2672,7 +2675,7 @@
       <c r="J59" s="27"/>
       <c r="K59" s="24"/>
     </row>
-    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="21"/>
       <c r="B60" s="35"/>
       <c r="C60" s="22">
@@ -2700,7 +2703,7 @@
       <c r="J60" s="27"/>
       <c r="K60" s="24"/>
     </row>
-    <row r="61" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="21"/>
       <c r="B61" s="40" t="s">
         <v>55</v>
@@ -2742,7 +2745,7 @@
         <v>313.72142639439198</v>
       </c>
     </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="21"/>
       <c r="B62" s="35"/>
       <c r="C62" s="22">
@@ -2770,7 +2773,7 @@
       <c r="J62" s="27"/>
       <c r="K62" s="24"/>
     </row>
-    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="21"/>
       <c r="B63" s="35" t="s">
         <v>43</v>
@@ -2800,7 +2803,7 @@
       <c r="J63" s="27"/>
       <c r="K63" s="24"/>
     </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="21"/>
       <c r="B64" s="35"/>
       <c r="C64" s="22">
@@ -2828,7 +2831,7 @@
       <c r="J64" s="27"/>
       <c r="K64" s="24"/>
     </row>
-    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="21"/>
       <c r="B65" s="35" t="s">
         <v>58</v>
@@ -2858,7 +2861,7 @@
       <c r="J65" s="27"/>
       <c r="K65" s="24"/>
     </row>
-    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66" s="21"/>
       <c r="B66" s="35"/>
       <c r="C66" s="22">
@@ -2886,7 +2889,7 @@
       <c r="J66" s="27"/>
       <c r="K66" s="24"/>
     </row>
-    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="21"/>
       <c r="B67" s="35" t="s">
         <v>59</v>
@@ -2920,7 +2923,7 @@
         <v>2.85</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="21"/>
       <c r="B68" s="35"/>
       <c r="C68" s="22">
@@ -2948,7 +2951,7 @@
       <c r="J68" s="27"/>
       <c r="K68" s="24"/>
     </row>
-    <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="21"/>
       <c r="B69" s="35"/>
       <c r="C69" s="22">
@@ -2976,7 +2979,7 @@
       <c r="J69" s="27"/>
       <c r="K69" s="24"/>
     </row>
-    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="21"/>
       <c r="B70" s="35" t="s">
         <v>24</v>
@@ -3001,7 +3004,7 @@
       </c>
       <c r="K70" s="24"/>
     </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="21"/>
       <c r="B71" s="35" t="s">
         <v>28</v>
@@ -3019,7 +3022,7 @@
       </c>
       <c r="K71" s="24"/>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="21"/>
       <c r="B72" s="35"/>
       <c r="C72" s="22"/>
@@ -3032,7 +3035,7 @@
       <c r="J72" s="27"/>
       <c r="K72" s="24"/>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
       <c r="A73" s="21">
         <v>7</v>
       </c>
@@ -3049,7 +3052,7 @@
       <c r="J73" s="27"/>
       <c r="K73" s="24"/>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="21"/>
       <c r="B74" s="35" t="s">
         <v>61</v>
@@ -3077,7 +3080,7 @@
       <c r="J74" s="27"/>
       <c r="K74" s="24"/>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="21"/>
       <c r="B75" s="35"/>
       <c r="C75" s="22">
@@ -3103,7 +3106,7 @@
       <c r="J75" s="27"/>
       <c r="K75" s="24"/>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="21"/>
       <c r="B76" s="35"/>
       <c r="C76" s="22">
@@ -3129,7 +3132,7 @@
       <c r="J76" s="27"/>
       <c r="K76" s="24"/>
     </row>
-    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="21"/>
       <c r="B77" s="35"/>
       <c r="C77" s="22">
@@ -3155,7 +3158,7 @@
       <c r="J77" s="27"/>
       <c r="K77" s="24"/>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="21"/>
       <c r="B78" s="35" t="s">
         <v>64</v>
@@ -3184,7 +3187,7 @@
       <c r="J78" s="27"/>
       <c r="K78" s="24"/>
     </row>
-    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="21"/>
       <c r="B79" s="35" t="s">
         <v>24</v>
@@ -3209,7 +3212,7 @@
       </c>
       <c r="K79" s="24"/>
     </row>
-    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A80" s="21"/>
       <c r="B80" s="35" t="s">
         <v>28</v>
@@ -3227,7 +3230,7 @@
       </c>
       <c r="K80" s="24"/>
     </row>
-    <row r="81" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A81" s="21"/>
       <c r="B81" s="35"/>
       <c r="C81" s="22"/>
@@ -3240,7 +3243,7 @@
       <c r="J81" s="27"/>
       <c r="K81" s="24"/>
     </row>
-    <row r="82" spans="1:31" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:31" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A82" s="21">
         <v>8</v>
       </c>
@@ -3269,7 +3272,7 @@
       </c>
       <c r="K82" s="24"/>
     </row>
-    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="21"/>
       <c r="B83" s="35"/>
       <c r="C83" s="22"/>
@@ -3282,7 +3285,7 @@
       <c r="J83" s="27"/>
       <c r="K83" s="24"/>
     </row>
-    <row r="84" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="21">
         <v>9</v>
       </c>
@@ -3311,7 +3314,7 @@
       </c>
       <c r="K84" s="24"/>
     </row>
-    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="21"/>
       <c r="B85" s="35"/>
       <c r="C85" s="22"/>
@@ -3324,7 +3327,7 @@
       <c r="J85" s="27"/>
       <c r="K85" s="24"/>
     </row>
-    <row r="86" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A86" s="9"/>
       <c r="B86" s="20" t="s">
         <v>16</v>
@@ -3345,7 +3348,7 @@
       <c r="P86" s="31"/>
       <c r="Q86" s="31"/>
     </row>
-    <row r="87" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
       <c r="M87" s="28"/>
       <c r="N87" s="29"/>
       <c r="O87" s="29"/>
@@ -3365,15 +3368,15 @@
       <c r="AD87" s="28"/>
       <c r="AE87" s="28"/>
     </row>
-    <row r="88" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B88" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C88" s="49">
+      <c r="C88" s="43">
         <f>J86</f>
         <v>489498.04796384519</v>
       </c>
-      <c r="D88" s="50"/>
+      <c r="D88" s="44"/>
       <c r="E88" s="10">
         <v>100</v>
       </c>
@@ -3403,14 +3406,14 @@
       <c r="AD88" s="12"/>
       <c r="AE88" s="12"/>
     </row>
-    <row r="89" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B89" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C89" s="52">
+      <c r="C89" s="47">
         <v>400000</v>
       </c>
-      <c r="D89" s="53"/>
+      <c r="D89" s="48"/>
       <c r="E89" s="10"/>
       <c r="M89" s="28"/>
       <c r="N89" s="29"/>
@@ -3432,15 +3435,15 @@
       <c r="AD89" s="28"/>
       <c r="AE89" s="28"/>
     </row>
-    <row r="90" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B90" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C90" s="52">
+      <c r="C90" s="47">
         <f>C89-C92-C93</f>
         <v>380000</v>
       </c>
-      <c r="D90" s="53"/>
+      <c r="D90" s="48"/>
       <c r="E90" s="10">
         <f>C90/C88*100</f>
         <v>77.63054450996853</v>
@@ -3465,15 +3468,15 @@
       <c r="AD90" s="28"/>
       <c r="AE90" s="28"/>
     </row>
-    <row r="91" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B91" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C91" s="54">
+      <c r="C91" s="49">
         <f>C88-C90</f>
         <v>109498.04796384519</v>
       </c>
-      <c r="D91" s="54"/>
+      <c r="D91" s="49"/>
       <c r="E91" s="10">
         <f>100-E90</f>
         <v>22.36945549003147</v>
@@ -3498,15 +3501,15 @@
       <c r="AD91" s="28"/>
       <c r="AE91" s="28"/>
     </row>
-    <row r="92" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B92" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C92" s="49">
+      <c r="C92" s="43">
         <f>C89*0.03</f>
         <v>12000</v>
       </c>
-      <c r="D92" s="50"/>
+      <c r="D92" s="44"/>
       <c r="E92" s="10">
         <v>3</v>
       </c>
@@ -3530,15 +3533,15 @@
       <c r="AD92" s="28"/>
       <c r="AE92" s="28"/>
     </row>
-    <row r="93" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
       <c r="B93" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C93" s="49">
+      <c r="C93" s="43">
         <f>C89*0.02</f>
         <v>8000</v>
       </c>
-      <c r="D93" s="50"/>
+      <c r="D93" s="44"/>
       <c r="E93" s="10">
         <v>2</v>
       </c>
@@ -3564,6 +3567,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C92:D92"/>
     <mergeCell ref="C93:D93"/>
     <mergeCell ref="A7:F7"/>
@@ -3572,13 +3582,2359 @@
     <mergeCell ref="C89:D89"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C91:D91"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;LPrepared By:
+Kristal Suwal&amp;CChecked By:
+Er. Milan Phuyal&amp;RApproved By:    
+Er. Prakash Singh Saud</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE93"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.109375" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+    </row>
+    <row r="5" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="46"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <v>1</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="24"/>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="22">
+        <v>6</v>
+      </c>
+      <c r="D10" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="E10" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="F10" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="G10" s="33">
+        <f>PRODUCT(C10:F10)</f>
+        <v>20.25</v>
+      </c>
+      <c r="H10" s="25"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+      <c r="B11" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="27">
+        <f>SUM(G10:G10)</f>
+        <v>20.25</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="26">
+        <v>663.31</v>
+      </c>
+      <c r="J11" s="27">
+        <f>G11*I11</f>
+        <v>13432.027499999998</v>
+      </c>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <v>2</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21"/>
+      <c r="B14" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="22">
+        <f>C10</f>
+        <v>6</v>
+      </c>
+      <c r="D14" s="23">
+        <f>D10</f>
+        <v>1.5</v>
+      </c>
+      <c r="E14" s="24">
+        <f>E10</f>
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G14" s="33">
+        <f>PRODUCT(C14:F14)</f>
+        <v>2.0249999999999999</v>
+      </c>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21"/>
+      <c r="B15" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="22">
+        <v>2</v>
+      </c>
+      <c r="D15" s="23">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="E15" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F15" s="24">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="33">
+        <f>PRODUCT(C15:F15)</f>
+        <v>2.786819199809456</v>
+      </c>
+      <c r="H15" s="25"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21"/>
+      <c r="B16" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="27">
+        <f>SUM(G14:G15)</f>
+        <v>4.8118191998094559</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="26">
+        <v>4473.1499999999996</v>
+      </c>
+      <c r="J16" s="27">
+        <f>G16*I16</f>
+        <v>21523.989053627665</v>
+      </c>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
+      <c r="B17" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="27">
+        <f>0.13*G16*3093.15</f>
+        <v>1934.8782125257806</v>
+      </c>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A19" s="21">
+        <v>3</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="22">
+        <f>C14</f>
+        <v>6</v>
+      </c>
+      <c r="D20" s="23">
+        <f>D14</f>
+        <v>1.5</v>
+      </c>
+      <c r="E20" s="24">
+        <f>E14</f>
+        <v>1.5</v>
+      </c>
+      <c r="F20" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="G20" s="33">
+        <f>PRODUCT(C20:F20)</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="27">
+        <f>SUM(G20:G20)</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I21" s="26">
+        <v>12983.1</v>
+      </c>
+      <c r="J21" s="27">
+        <f>G21*I21</f>
+        <v>8763.5925000000007</v>
+      </c>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="27">
+        <f>0.13*G21*8078.11</f>
+        <v>708.85415250000005</v>
+      </c>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A24" s="21">
+        <v>4</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="35" t="str">
+        <f>B20</f>
+        <v>;-for footing</v>
+      </c>
+      <c r="C25" s="22">
+        <f>C20</f>
+        <v>6</v>
+      </c>
+      <c r="D25" s="23">
+        <f>D20*4</f>
+        <v>6</v>
+      </c>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24">
+        <f>0.23</f>
+        <v>0.23</v>
+      </c>
+      <c r="G25" s="33">
+        <f>PRODUCT(C25:F25)</f>
+        <v>8.2800000000000011</v>
+      </c>
+      <c r="H25" s="25"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21"/>
+      <c r="B26" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="22">
+        <v>6</v>
+      </c>
+      <c r="D26" s="23">
+        <f>0.3*4</f>
+        <v>1.2</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G26" s="33">
+        <f>PRODUCT(C26:F26)</f>
+        <v>7.6805851874428512</v>
+      </c>
+      <c r="H26" s="25"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="24"/>
+    </row>
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21"/>
+      <c r="B27" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="22">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="D27" s="23">
+        <f>9.667/3.281</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24">
+        <f>0.23*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G27" s="33">
+        <f t="shared" ref="G27:G32" si="0">PRODUCT(C27:F27)</f>
+        <v>10.842596769277659</v>
+      </c>
+      <c r="H27" s="25"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="24"/>
+    </row>
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="22">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="D28" s="23">
+        <f>9.5/3.281</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24">
+        <f>0.23*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G28" s="33">
+        <f t="shared" si="0"/>
+        <v>7.9914660164583964</v>
+      </c>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="24"/>
+    </row>
+    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21"/>
+      <c r="B29" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="22">
+        <f>C26</f>
+        <v>6</v>
+      </c>
+      <c r="D29" s="23">
+        <f>0.3*4</f>
+        <v>1.2</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24">
+        <f>8.17/3.281</f>
+        <v>2.4900944833892105</v>
+      </c>
+      <c r="G29" s="33">
+        <f t="shared" si="0"/>
+        <v>17.928680280402315</v>
+      </c>
+      <c r="H29" s="25"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="24"/>
+    </row>
+    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21"/>
+      <c r="B30" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="22">
+        <f>0*4</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="23">
+        <f>9.667/3.281</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24">
+        <f>0.23*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G30" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="25"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="24"/>
+    </row>
+    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="21"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="22">
+        <f>0*3</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="23">
+        <f>9.5/3.281</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24">
+        <f>0.23*2</f>
+        <v>0.46</v>
+      </c>
+      <c r="G31" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="25"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="24"/>
+    </row>
+    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21"/>
+      <c r="B32" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="22">
+        <f>0*1</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="23">
+        <f>(22.333+3)/3.281</f>
+        <v>7.7211216092654666</v>
+      </c>
+      <c r="E32" s="24">
+        <f>(11.5+3)/3.281</f>
+        <v>4.4193843340444987</v>
+      </c>
+      <c r="F32" s="24"/>
+      <c r="G32" s="33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="25"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="24"/>
+    </row>
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21"/>
+      <c r="B33" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="27">
+        <f>SUM(G25:G32)</f>
+        <v>52.723328253581229</v>
+      </c>
+      <c r="H33" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="26">
+        <v>915.42</v>
+      </c>
+      <c r="J33" s="27">
+        <f>G33*I33</f>
+        <v>48263.989149893328</v>
+      </c>
+      <c r="K33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="21"/>
+      <c r="B34" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="27">
+        <f>0.13*G33*46827.87/100</f>
+        <v>3209.5975098538374</v>
+      </c>
+      <c r="K34" s="24"/>
+    </row>
+    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="24"/>
+    </row>
+    <row r="36" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A36" s="21">
+        <v>5</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="22"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="24"/>
+    </row>
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="21"/>
+      <c r="B37" s="35" t="str">
+        <f>B25</f>
+        <v>;-for footing</v>
+      </c>
+      <c r="C37" s="22">
+        <f>C25</f>
+        <v>6</v>
+      </c>
+      <c r="D37" s="23">
+        <f>1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="E37" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="F37" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="G37" s="33">
+        <f>PRODUCT(C37:F37)</f>
+        <v>3.105</v>
+      </c>
+      <c r="H37" s="25"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="24"/>
+    </row>
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="21"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="22">
+        <v>6</v>
+      </c>
+      <c r="D38" s="23">
+        <f>1.667/3.281</f>
+        <v>0.50807680585187442</v>
+      </c>
+      <c r="E38" s="24">
+        <f>1.667/3.281</f>
+        <v>0.50807680585187442</v>
+      </c>
+      <c r="F38" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="G38" s="33">
+        <f>(F38/3)*((D37*E37)+(D38*E38)+(SQRT((D37*E37)*(D38*E38))))</f>
+        <v>0.25071972245572161</v>
+      </c>
+      <c r="H38" s="25"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="24"/>
+    </row>
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="21"/>
+      <c r="B39" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="22">
+        <v>6</v>
+      </c>
+      <c r="D39" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E39" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F39" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="G39" s="33">
+        <f>PRODUCT(C39:F39)</f>
+        <v>0.80999999999999983</v>
+      </c>
+      <c r="H39" s="25"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="24"/>
+    </row>
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="21"/>
+      <c r="B40" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="22">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="D40" s="23">
+        <f>D27</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="E40" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F40" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="G40" s="33">
+        <f t="shared" ref="G40:G46" si="1">PRODUCT(C40:F40)</f>
+        <v>1.2468986284669308</v>
+      </c>
+      <c r="H40" s="25"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="24"/>
+    </row>
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="21"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="22">
+        <f>2*3</f>
+        <v>6</v>
+      </c>
+      <c r="D41" s="23">
+        <f>D28</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="E41" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F41" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="G41" s="33">
+        <f t="shared" si="1"/>
+        <v>0.91901859189271562</v>
+      </c>
+      <c r="H41" s="25"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="21"/>
+      <c r="B42" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="22">
+        <v>2</v>
+      </c>
+      <c r="D42" s="23">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="E42" s="24">
+        <f>10/3.281</f>
+        <v>3.047851264858275</v>
+      </c>
+      <c r="F42" s="24">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G42" s="33">
+        <f t="shared" si="1"/>
+        <v>1.393409599904728</v>
+      </c>
+      <c r="H42" s="25"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="21"/>
+      <c r="B43" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="22">
+        <f>C39</f>
+        <v>6</v>
+      </c>
+      <c r="D43" s="23">
+        <v>0.3</v>
+      </c>
+      <c r="E43" s="24">
+        <v>0.3</v>
+      </c>
+      <c r="F43" s="24">
+        <f>8.917/3.281</f>
+        <v>2.7177689728741234</v>
+      </c>
+      <c r="G43" s="33">
+        <f t="shared" si="1"/>
+        <v>1.4675952453520265</v>
+      </c>
+      <c r="H43" s="25"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="24"/>
+    </row>
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="21"/>
+      <c r="B44" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="22">
+        <f>0*4</f>
+        <v>0</v>
+      </c>
+      <c r="D44" s="23">
+        <f>D40</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="E44" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F44" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="G44" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="25"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="24"/>
+    </row>
+    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="21"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="22">
+        <f>0*3</f>
+        <v>0</v>
+      </c>
+      <c r="D45" s="23">
+        <f>D41</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="E45" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F45" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="G45" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="25"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="24"/>
+    </row>
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="22">
+        <f>0*1</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="23">
+        <f>D32</f>
+        <v>7.7211216092654666</v>
+      </c>
+      <c r="E46" s="24">
+        <f>E32</f>
+        <v>4.4193843340444987</v>
+      </c>
+      <c r="F46" s="24">
+        <f>5/12/3.281</f>
+        <v>0.12699380270242813</v>
+      </c>
+      <c r="G46" s="33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="25"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="24"/>
+    </row>
+    <row r="47" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="27">
+        <f>SUM(G37:G46)</f>
+        <v>9.1926417880721214</v>
+      </c>
+      <c r="H47" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I47" s="26">
+        <v>13568.9</v>
+      </c>
+      <c r="J47" s="27">
+        <f>G47*I47</f>
+        <v>124734.03715817181</v>
+      </c>
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="21"/>
+      <c r="B48" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="27"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="27">
+        <f>0.13*G47*9524.2</f>
+        <v>11381.832659334344</v>
+      </c>
+      <c r="K48" s="24"/>
+    </row>
+    <row r="49" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="21"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="23"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="24"/>
+    </row>
+    <row r="50" spans="1:15" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="21">
+        <v>6</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="F50" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="H50" s="25"/>
+      <c r="I50" s="26"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="24"/>
+    </row>
+    <row r="51" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="22">
+        <f>6*2*10</f>
+        <v>120</v>
+      </c>
+      <c r="D51" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="E51" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F51" s="24">
+        <f>PRODUCT(C51:E51)</f>
+        <v>160</v>
+      </c>
+      <c r="G51" s="27">
+        <f>F51/1000</f>
+        <v>0.16</v>
+      </c>
+      <c r="H51" s="25"/>
+      <c r="I51" s="26"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="24"/>
+    </row>
+    <row r="52" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="21"/>
+      <c r="B52" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" s="22">
+        <f>6*8</f>
+        <v>48</v>
+      </c>
+      <c r="D52" s="23">
+        <f>13.917/3.281+0.72*2</f>
+        <v>5.6816946053032602</v>
+      </c>
+      <c r="E52" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F52" s="24">
+        <f>PRODUCT(C52:E52)</f>
+        <v>242.41896982627242</v>
+      </c>
+      <c r="G52" s="27">
+        <f>F52/1000</f>
+        <v>0.24241896982627242</v>
+      </c>
+      <c r="H52" s="25"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="24"/>
+    </row>
+    <row r="53" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="21"/>
+      <c r="B53" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C53" s="22">
+        <f>6*15</f>
+        <v>90</v>
+      </c>
+      <c r="D53" s="23">
+        <f>(0.23*4+0.05*2)</f>
+        <v>1.02</v>
+      </c>
+      <c r="E53" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F53" s="24">
+        <f t="shared" ref="F53:F54" si="2">PRODUCT(C53:E53)</f>
+        <v>36.266666666666666</v>
+      </c>
+      <c r="G53" s="27">
+        <f t="shared" ref="G53:G54" si="3">F53/1000</f>
+        <v>3.6266666666666662E-2</v>
+      </c>
+      <c r="H53" s="25"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="24"/>
+      <c r="M53" s="1">
+        <f>12*60</f>
+        <v>720</v>
+      </c>
+      <c r="N53" s="1">
+        <f>1.333/3.281*1000</f>
+        <v>406.27857360560802</v>
+      </c>
+      <c r="O53" s="1">
+        <f>M53-N53</f>
+        <v>313.72142639439198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
+      <c r="B54" s="35"/>
+      <c r="C54" s="22">
+        <f>C53</f>
+        <v>90</v>
+      </c>
+      <c r="D54" s="23">
+        <f>0.15*4+0.05*2</f>
+        <v>0.7</v>
+      </c>
+      <c r="E54" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F54" s="24">
+        <f t="shared" si="2"/>
+        <v>24.888888888888886</v>
+      </c>
+      <c r="G54" s="27">
+        <f t="shared" si="3"/>
+        <v>2.4888888888888884E-2</v>
+      </c>
+      <c r="H54" s="25"/>
+      <c r="I54" s="26"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="24"/>
+    </row>
+    <row r="55" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="22">
+        <f>5*C40</f>
+        <v>40</v>
+      </c>
+      <c r="D55" s="23">
+        <f>D40+0.72</f>
+        <v>3.6663578177384943</v>
+      </c>
+      <c r="E55" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F55" s="24">
+        <f>PRODUCT(C55:E55)</f>
+        <v>130.35938907514645</v>
+      </c>
+      <c r="G55" s="27">
+        <f>F55/1000</f>
+        <v>0.13035938907514646</v>
+      </c>
+      <c r="H55" s="25"/>
+      <c r="I55" s="26"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="24"/>
+    </row>
+    <row r="56" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="21"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="22">
+        <f>5*C41</f>
+        <v>30</v>
+      </c>
+      <c r="D56" s="23">
+        <f>D41+2*0.72</f>
+        <v>4.3354587016153605</v>
+      </c>
+      <c r="E56" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F56" s="24">
+        <f>PRODUCT(C56:E56)</f>
+        <v>115.61223204307626</v>
+      </c>
+      <c r="G56" s="27">
+        <f>F56/1000</f>
+        <v>0.11561223204307626</v>
+      </c>
+      <c r="H56" s="25"/>
+      <c r="I56" s="26"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="24"/>
+    </row>
+    <row r="57" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="21"/>
+      <c r="B57" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="22">
+        <f>8*TRUNC((D55-2*0.72)/0.125,0)</f>
+        <v>136</v>
+      </c>
+      <c r="D57" s="23">
+        <f>(0.15*4+0.05*2)</f>
+        <v>0.7</v>
+      </c>
+      <c r="E57" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F57" s="24">
+        <f t="shared" ref="F57:F63" si="4">PRODUCT(C57:E57)</f>
+        <v>37.609876543209872</v>
+      </c>
+      <c r="G57" s="41">
+        <f t="shared" ref="G57:G63" si="5">F57/1000</f>
+        <v>3.7609876543209873E-2</v>
+      </c>
+      <c r="H57" s="25"/>
+      <c r="I57" s="26"/>
+      <c r="J57" s="41"/>
+      <c r="K57" s="24"/>
+      <c r="M57" s="42">
+        <f>12*60</f>
+        <v>720</v>
+      </c>
+      <c r="N57" s="42">
+        <f>1.333/3.281*1000</f>
+        <v>406.27857360560802</v>
+      </c>
+      <c r="O57" s="42">
+        <f>M57-N57</f>
+        <v>313.72142639439198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="21"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="22">
+        <f>6*TRUNC((D56-2*0.72)/0.125,0)</f>
+        <v>138</v>
+      </c>
+      <c r="D58" s="23">
+        <f>(0.15*4+0.05*2)</f>
+        <v>0.7</v>
+      </c>
+      <c r="E58" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F58" s="24">
+        <f t="shared" si="4"/>
+        <v>38.162962962962958</v>
+      </c>
+      <c r="G58" s="41">
+        <f t="shared" si="5"/>
+        <v>3.8162962962962961E-2</v>
+      </c>
+      <c r="H58" s="25"/>
+      <c r="I58" s="26"/>
+      <c r="J58" s="41"/>
+      <c r="K58" s="24"/>
+    </row>
+    <row r="59" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21"/>
+      <c r="B59" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C59" s="22">
+        <f>0*2</f>
+        <v>0</v>
+      </c>
+      <c r="D59" s="23">
+        <f>(20.333/3.281)+0.72*2</f>
+        <v>7.6371959768363293</v>
+      </c>
+      <c r="E59" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F59" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G59" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H59" s="25"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="27"/>
+      <c r="K59" s="24"/>
+    </row>
+    <row r="60" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="21"/>
+      <c r="B60" s="35"/>
+      <c r="C60" s="22">
+        <f>0*3</f>
+        <v>0</v>
+      </c>
+      <c r="D60" s="23">
+        <f>(9.5/3.281)+0.72*2</f>
+        <v>4.3354587016153605</v>
+      </c>
+      <c r="E60" s="24">
+        <f>12*12/162</f>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="F60" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G60" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H60" s="25"/>
+      <c r="I60" s="26"/>
+      <c r="J60" s="27"/>
+      <c r="K60" s="24"/>
+    </row>
+    <row r="61" spans="1:15" s="42" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="21"/>
+      <c r="B61" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="22">
+        <f>0*2*TRUNC((D59-3*0.72)/0.125,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D61" s="23">
+        <f>(0.23*2+0.15*2+0.05*2)</f>
+        <v>0.86</v>
+      </c>
+      <c r="E61" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F61" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G61" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H61" s="25"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="41"/>
+      <c r="K61" s="24"/>
+      <c r="M61" s="42">
+        <f>12*60</f>
+        <v>720</v>
+      </c>
+      <c r="N61" s="42">
+        <f>1.333/3.281*1000</f>
+        <v>406.27857360560802</v>
+      </c>
+      <c r="O61" s="42">
+        <f>M61-N61</f>
+        <v>313.72142639439198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="21"/>
+      <c r="B62" s="35"/>
+      <c r="C62" s="22">
+        <f>0*3*TRUNC((D60-2*0.72)/0.125,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D62" s="23">
+        <f>(0.23*2+0.15*2+0.05*2)</f>
+        <v>0.86</v>
+      </c>
+      <c r="E62" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F62" s="24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G62" s="41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="25"/>
+      <c r="I62" s="26"/>
+      <c r="J62" s="27"/>
+      <c r="K62" s="24"/>
+    </row>
+    <row r="63" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="21"/>
+      <c r="B63" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="22">
+        <f>0*TRUNC(12.5/0.5,0)+1</f>
+        <v>1</v>
+      </c>
+      <c r="D63" s="23">
+        <f>25/3.281</f>
+        <v>7.6196281621456867</v>
+      </c>
+      <c r="E63" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F63" s="24">
+        <f t="shared" si="4"/>
+        <v>3.0102234714649625</v>
+      </c>
+      <c r="G63" s="41">
+        <f t="shared" si="5"/>
+        <v>3.0102234714649624E-3</v>
+      </c>
+      <c r="H63" s="25"/>
+      <c r="I63" s="26"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="24"/>
+    </row>
+    <row r="64" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="21"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="22">
+        <f>0*TRUNC((25.333-0.333-0.75*3)/0.5,0)+1</f>
+        <v>1</v>
+      </c>
+      <c r="D64" s="23">
+        <f>14.17/3.281</f>
+        <v>4.3188052423041752</v>
+      </c>
+      <c r="E64" s="24">
+        <f>8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F64" s="24">
+        <f>PRODUCT(C64:E64)</f>
+        <v>1.7061946636263408</v>
+      </c>
+      <c r="G64" s="41">
+        <f>F64/1000</f>
+        <v>1.7061946636263408E-3</v>
+      </c>
+      <c r="H64" s="25"/>
+      <c r="I64" s="26"/>
+      <c r="J64" s="27"/>
+      <c r="K64" s="24"/>
+    </row>
+    <row r="65" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="21"/>
+      <c r="B65" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" s="22">
+        <f>0*30</f>
+        <v>0</v>
+      </c>
+      <c r="D65" s="23">
+        <f>14.17/3.281</f>
+        <v>4.3188052423041752</v>
+      </c>
+      <c r="E65" s="24">
+        <f t="shared" ref="E65:E69" si="6">8*8/162</f>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F65" s="24">
+        <f t="shared" ref="F65:F69" si="7">PRODUCT(C65:E65)</f>
+        <v>0</v>
+      </c>
+      <c r="G65" s="41">
+        <f t="shared" ref="G65:G69" si="8">F65/1000</f>
+        <v>0</v>
+      </c>
+      <c r="H65" s="25"/>
+      <c r="I65" s="26"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="24"/>
+    </row>
+    <row r="66" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="21"/>
+      <c r="B66" s="35"/>
+      <c r="C66" s="22">
+        <f>0*9*2</f>
+        <v>0</v>
+      </c>
+      <c r="D66" s="23">
+        <f>25/3.281</f>
+        <v>7.6196281621456867</v>
+      </c>
+      <c r="E66" s="24">
+        <f t="shared" si="6"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F66" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G66" s="41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H66" s="25"/>
+      <c r="I66" s="26"/>
+      <c r="J66" s="27"/>
+      <c r="K66" s="24"/>
+    </row>
+    <row r="67" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="21"/>
+      <c r="B67" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="22">
+        <f>0*7*4</f>
+        <v>0</v>
+      </c>
+      <c r="D67" s="23">
+        <f>1.5</f>
+        <v>1.5</v>
+      </c>
+      <c r="E67" s="24">
+        <f t="shared" si="6"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F67" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G67" s="41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H67" s="25"/>
+      <c r="I67" s="26"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="24"/>
+      <c r="O67" s="1">
+        <f>9.5*0.3</f>
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="21"/>
+      <c r="B68" s="35"/>
+      <c r="C68" s="22">
+        <f>0*16</f>
+        <v>0</v>
+      </c>
+      <c r="D68" s="23">
+        <f>5.333/3.281</f>
+        <v>1.6254190795489181</v>
+      </c>
+      <c r="E68" s="24">
+        <f t="shared" si="6"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F68" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G68" s="41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H68" s="25"/>
+      <c r="I68" s="26"/>
+      <c r="J68" s="27"/>
+      <c r="K68" s="24"/>
+    </row>
+    <row r="69" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="21"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="22">
+        <f>0*8</f>
+        <v>0</v>
+      </c>
+      <c r="D69" s="23">
+        <f>7.25/3.281</f>
+        <v>2.2096921670222494</v>
+      </c>
+      <c r="E69" s="24">
+        <f t="shared" si="6"/>
+        <v>0.39506172839506171</v>
+      </c>
+      <c r="F69" s="24">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G69" s="41">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="H69" s="25"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="24"/>
+    </row>
+    <row r="70" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="21"/>
+      <c r="B70" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C70" s="22"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="27">
+        <f>SUM(G51:G69)</f>
+        <v>0.7900354041413149</v>
+      </c>
+      <c r="H70" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I70" s="26">
+        <v>131940</v>
+      </c>
+      <c r="J70" s="27">
+        <f>G70*I70</f>
+        <v>104237.27122240509</v>
+      </c>
+      <c r="K70" s="24"/>
+    </row>
+    <row r="71" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="21"/>
+      <c r="B71" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C71" s="22"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="25"/>
+      <c r="I71" s="26"/>
+      <c r="J71" s="27">
+        <f>0.13*G70*106200</f>
+        <v>10907.228789574994</v>
+      </c>
+      <c r="K71" s="24"/>
+    </row>
+    <row r="72" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="21"/>
+      <c r="B72" s="35"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="23"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="27"/>
+      <c r="H72" s="25"/>
+      <c r="I72" s="26"/>
+      <c r="J72" s="27"/>
+      <c r="K72" s="24"/>
+    </row>
+    <row r="73" spans="1:15" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.3">
+      <c r="A73" s="21">
+        <v>7</v>
+      </c>
+      <c r="B73" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C73" s="22"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="27"/>
+      <c r="H73" s="25"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="27"/>
+      <c r="K73" s="24"/>
+    </row>
+    <row r="74" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="21"/>
+      <c r="B74" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C74" s="22">
+        <v>4</v>
+      </c>
+      <c r="D74" s="23">
+        <f>D27</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="E74" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F74" s="24">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G74" s="33">
+        <f>PRODUCT(C74:F74)</f>
+        <v>2.8915794492892259</v>
+      </c>
+      <c r="H74" s="25"/>
+      <c r="I74" s="26"/>
+      <c r="J74" s="27"/>
+      <c r="K74" s="24"/>
+    </row>
+    <row r="75" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="21"/>
+      <c r="B75" s="35"/>
+      <c r="C75" s="22">
+        <v>3</v>
+      </c>
+      <c r="D75" s="23">
+        <f>D28</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="E75" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F75" s="24">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G75" s="33">
+        <f>PRODUCT(C75:F75)</f>
+        <v>2.1312199830542808</v>
+      </c>
+      <c r="H75" s="25"/>
+      <c r="I75" s="26"/>
+      <c r="J75" s="27"/>
+      <c r="K75" s="24"/>
+    </row>
+    <row r="76" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="21"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="22">
+        <f>0*1</f>
+        <v>0</v>
+      </c>
+      <c r="D76" s="23">
+        <f>D74</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="E76" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F76" s="24">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G76" s="33">
+        <f>PRODUCT(C76:F76)</f>
+        <v>0</v>
+      </c>
+      <c r="H76" s="25"/>
+      <c r="I76" s="26"/>
+      <c r="J76" s="27"/>
+      <c r="K76" s="24"/>
+    </row>
+    <row r="77" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="21"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="22">
+        <f>0*2</f>
+        <v>0</v>
+      </c>
+      <c r="D77" s="23">
+        <f>D75</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="E77" s="24">
+        <v>0.23</v>
+      </c>
+      <c r="F77" s="24">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G77" s="33">
+        <f>PRODUCT(C77:F77)</f>
+        <v>0</v>
+      </c>
+      <c r="H77" s="25"/>
+      <c r="I77" s="26"/>
+      <c r="J77" s="27"/>
+      <c r="K77" s="24"/>
+    </row>
+    <row r="78" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="21"/>
+      <c r="B78" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" s="22">
+        <f>0*2*0.5</f>
+        <v>0</v>
+      </c>
+      <c r="D78" s="23">
+        <f>D77+0.45*2+0.6</f>
+        <v>4.395458701615361</v>
+      </c>
+      <c r="E78" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="F78" s="24">
+        <f>3.5/3.281</f>
+        <v>1.0667479427003961</v>
+      </c>
+      <c r="G78" s="33">
+        <f>PRODUCT(C78:F78)</f>
+        <v>0</v>
+      </c>
+      <c r="H78" s="25"/>
+      <c r="I78" s="26"/>
+      <c r="J78" s="27"/>
+      <c r="K78" s="24"/>
+    </row>
+    <row r="79" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="21"/>
+      <c r="B79" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="23"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="27">
+        <f>SUM(G74:G78)</f>
+        <v>5.0227994323435068</v>
+      </c>
+      <c r="H79" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="I79" s="26">
+        <v>14362.76</v>
+      </c>
+      <c r="J79" s="27">
+        <f>G79*I79</f>
+        <v>72141.262774886025</v>
+      </c>
+      <c r="K79" s="24"/>
+    </row>
+    <row r="80" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="21"/>
+      <c r="B80" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C80" s="22"/>
+      <c r="D80" s="23"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="27"/>
+      <c r="H80" s="25"/>
+      <c r="I80" s="26"/>
+      <c r="J80" s="27">
+        <f>0.13*G79*10311.74</f>
+        <v>6733.1942364015986</v>
+      </c>
+      <c r="K80" s="24"/>
+    </row>
+    <row r="81" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="21"/>
+      <c r="B81" s="35"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="27"/>
+      <c r="H81" s="25"/>
+      <c r="I81" s="26"/>
+      <c r="J81" s="27"/>
+      <c r="K81" s="24"/>
+    </row>
+    <row r="82" spans="1:31" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="21">
+        <v>8</v>
+      </c>
+      <c r="B82" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C82" s="22">
+        <v>1</v>
+      </c>
+      <c r="D82" s="23"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="33">
+        <f>PRODUCT(C82:F82)</f>
+        <v>1</v>
+      </c>
+      <c r="H82" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" s="26">
+        <v>20000</v>
+      </c>
+      <c r="J82" s="27">
+        <f>G82*I82</f>
+        <v>20000</v>
+      </c>
+      <c r="K82" s="24"/>
+    </row>
+    <row r="83" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="21"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="23"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="27"/>
+      <c r="H83" s="25"/>
+      <c r="I83" s="26"/>
+      <c r="J83" s="27"/>
+      <c r="K83" s="24"/>
+    </row>
+    <row r="84" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="21">
+        <v>9</v>
+      </c>
+      <c r="B84" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84" s="22">
+        <v>1</v>
+      </c>
+      <c r="D84" s="23"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="33">
+        <f>PRODUCT(C84:F84)</f>
+        <v>1</v>
+      </c>
+      <c r="H84" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I84" s="26">
+        <v>500</v>
+      </c>
+      <c r="J84" s="27">
+        <f>G84*I84</f>
+        <v>500</v>
+      </c>
+      <c r="K84" s="24"/>
+    </row>
+    <row r="85" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="21"/>
+      <c r="B85" s="35"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="27"/>
+      <c r="H85" s="25"/>
+      <c r="I85" s="26"/>
+      <c r="J85" s="27"/>
+      <c r="K85" s="24"/>
+    </row>
+    <row r="86" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A86" s="9"/>
+      <c r="B86" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86" s="8"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="7"/>
+      <c r="I86" s="7"/>
+      <c r="J86" s="7">
+        <f>SUM(J9:J85)</f>
+        <v>448471.75491917448</v>
+      </c>
+      <c r="K86" s="4"/>
+      <c r="M86" s="28"/>
+      <c r="P86" s="31"/>
+      <c r="Q86" s="31"/>
+    </row>
+    <row r="87" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="M87" s="28"/>
+      <c r="N87" s="29"/>
+      <c r="O87" s="29"/>
+      <c r="P87" s="30"/>
+      <c r="R87" s="29"/>
+      <c r="S87" s="29"/>
+      <c r="T87" s="29"/>
+      <c r="U87" s="28"/>
+      <c r="V87" s="28"/>
+      <c r="W87" s="28"/>
+      <c r="X87" s="28"/>
+      <c r="Y87" s="28"/>
+      <c r="Z87" s="28"/>
+      <c r="AA87" s="28"/>
+      <c r="AB87" s="28"/>
+      <c r="AC87" s="28"/>
+      <c r="AD87" s="28"/>
+      <c r="AE87" s="28"/>
+    </row>
+    <row r="88" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B88" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="43">
+        <f>J86</f>
+        <v>448471.75491917448</v>
+      </c>
+      <c r="D88" s="44"/>
+      <c r="E88" s="10">
+        <v>100</v>
+      </c>
+      <c r="F88" s="12"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="16"/>
+      <c r="M88" s="12"/>
+      <c r="N88" s="29"/>
+      <c r="O88" s="29"/>
+      <c r="P88" s="29"/>
+      <c r="Q88" s="29"/>
+      <c r="R88" s="29"/>
+      <c r="S88" s="29"/>
+      <c r="T88" s="29"/>
+      <c r="U88" s="12"/>
+      <c r="V88" s="12"/>
+      <c r="W88" s="12"/>
+      <c r="X88" s="12"/>
+      <c r="Y88" s="12"/>
+      <c r="Z88" s="12"/>
+      <c r="AA88" s="12"/>
+      <c r="AB88" s="12"/>
+      <c r="AC88" s="12"/>
+      <c r="AD88" s="12"/>
+      <c r="AE88" s="12"/>
+    </row>
+    <row r="89" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B89" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" s="47">
+        <v>400000</v>
+      </c>
+      <c r="D89" s="48"/>
+      <c r="E89" s="10"/>
+      <c r="M89" s="28"/>
+      <c r="N89" s="29"/>
+      <c r="O89" s="29"/>
+      <c r="P89" s="29"/>
+      <c r="Q89" s="29"/>
+      <c r="R89" s="29"/>
+      <c r="S89" s="29"/>
+      <c r="T89" s="29"/>
+      <c r="U89" s="28"/>
+      <c r="V89" s="28"/>
+      <c r="W89" s="28"/>
+      <c r="X89" s="28"/>
+      <c r="Y89" s="28"/>
+      <c r="Z89" s="28"/>
+      <c r="AA89" s="28"/>
+      <c r="AB89" s="28"/>
+      <c r="AC89" s="28"/>
+      <c r="AD89" s="28"/>
+      <c r="AE89" s="28"/>
+    </row>
+    <row r="90" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B90" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C90" s="47">
+        <f>C89-C92-C93</f>
+        <v>380000</v>
+      </c>
+      <c r="D90" s="48"/>
+      <c r="E90" s="10">
+        <f>C90/C88*100</f>
+        <v>84.732203495956</v>
+      </c>
+      <c r="M90" s="28"/>
+      <c r="N90" s="28"/>
+      <c r="O90" s="28"/>
+      <c r="P90" s="28"/>
+      <c r="Q90" s="28"/>
+      <c r="R90" s="28"/>
+      <c r="S90" s="28"/>
+      <c r="T90" s="28"/>
+      <c r="U90" s="28"/>
+      <c r="V90" s="28"/>
+      <c r="W90" s="28"/>
+      <c r="X90" s="28"/>
+      <c r="Y90" s="28"/>
+      <c r="Z90" s="28"/>
+      <c r="AA90" s="28"/>
+      <c r="AB90" s="28"/>
+      <c r="AC90" s="28"/>
+      <c r="AD90" s="28"/>
+      <c r="AE90" s="28"/>
+    </row>
+    <row r="91" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B91" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" s="49">
+        <f>C88-C90</f>
+        <v>68471.754919174477</v>
+      </c>
+      <c r="D91" s="49"/>
+      <c r="E91" s="10">
+        <f>100-E90</f>
+        <v>15.267796504044</v>
+      </c>
+      <c r="M91" s="28"/>
+      <c r="N91" s="28"/>
+      <c r="O91" s="28"/>
+      <c r="P91" s="28"/>
+      <c r="Q91" s="28"/>
+      <c r="R91" s="28"/>
+      <c r="S91" s="28"/>
+      <c r="T91" s="28"/>
+      <c r="U91" s="28"/>
+      <c r="V91" s="28"/>
+      <c r="W91" s="28"/>
+      <c r="X91" s="28"/>
+      <c r="Y91" s="28"/>
+      <c r="Z91" s="28"/>
+      <c r="AA91" s="28"/>
+      <c r="AB91" s="28"/>
+      <c r="AC91" s="28"/>
+      <c r="AD91" s="28"/>
+      <c r="AE91" s="28"/>
+    </row>
+    <row r="92" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B92" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C92" s="43">
+        <f>C89*0.03</f>
+        <v>12000</v>
+      </c>
+      <c r="D92" s="44"/>
+      <c r="E92" s="10">
+        <v>3</v>
+      </c>
+      <c r="M92" s="28"/>
+      <c r="N92" s="28"/>
+      <c r="O92" s="28"/>
+      <c r="P92" s="28"/>
+      <c r="Q92" s="28"/>
+      <c r="R92" s="28"/>
+      <c r="S92" s="28"/>
+      <c r="T92" s="28"/>
+      <c r="U92" s="28"/>
+      <c r="V92" s="28"/>
+      <c r="W92" s="28"/>
+      <c r="X92" s="28"/>
+      <c r="Y92" s="28"/>
+      <c r="Z92" s="28"/>
+      <c r="AA92" s="28"/>
+      <c r="AB92" s="28"/>
+      <c r="AC92" s="28"/>
+      <c r="AD92" s="28"/>
+      <c r="AE92" s="28"/>
+    </row>
+    <row r="93" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="B93" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="43">
+        <f>C89*0.02</f>
+        <v>8000</v>
+      </c>
+      <c r="D93" s="44"/>
+      <c r="E93" s="10">
+        <v>2</v>
+      </c>
+      <c r="M93" s="28"/>
+      <c r="N93" s="28"/>
+      <c r="O93" s="28"/>
+      <c r="P93" s="28"/>
+      <c r="Q93" s="28"/>
+      <c r="R93" s="28"/>
+      <c r="S93" s="28"/>
+      <c r="T93" s="28"/>
+      <c r="U93" s="28"/>
+      <c r="V93" s="28"/>
+      <c r="W93" s="28"/>
+      <c r="X93" s="28"/>
+      <c r="Y93" s="28"/>
+      <c r="Z93" s="28"/>
+      <c r="AA93" s="28"/>
+      <c r="AB93" s="28"/>
+      <c r="AC93" s="28"/>
+      <c r="AD93" s="28"/>
+      <c r="AE93" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>